<commit_message>
satrt an above ground c analysis
</commit_message>
<xml_diff>
--- a/code_for_stats/c_lm_model_results.xlsx
+++ b/code_for_stats/c_lm_model_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmersonEmmerson/Documents/Master's/C_forecasting_NL/code_for_stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B6889D-84E9-814A-A0F5-ED3CEE492C1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D867E745-3D58-0043-8EDC-0CB3CC30EEC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16940" activeTab="3" xr2:uid="{2A789B6C-DF01-8A4C-BB45-45F2C6B1CDE0}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16940" xr2:uid="{2A789B6C-DF01-8A4C-BB45-45F2C6B1CDE0}"/>
   </bookViews>
   <sheets>
     <sheet name="by site" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="103">
   <si>
     <t>park</t>
   </si>
@@ -123,9 +123,6 @@
     <t>**</t>
   </si>
   <si>
-    <t>*** (as intercept)</t>
-  </si>
-  <si>
     <t>P values (significance)</t>
   </si>
   <si>
@@ -349,6 +346,9 @@
   </si>
   <si>
     <t>don't get sig values from mixed models</t>
+  </si>
+  <si>
+    <t>thurd after ecoevo</t>
   </si>
 </sst>
 </file>
@@ -915,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22840F77-1CD5-7545-896A-C96C00E42A18}">
   <dimension ref="A1:AN47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -944,12 +944,12 @@
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1065,7 +1065,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>22</v>
@@ -1075,7 +1075,7 @@
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>26</v>
@@ -1091,7 +1091,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9" t="s">
@@ -1099,7 +1099,7 @@
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>24</v>
@@ -1113,14 +1113,14 @@
         <v>7</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>24</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -1132,16 +1132,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I10" s="9"/>
       <c r="AJ10" s="16"/>
@@ -1151,12 +1151,12 @@
         <v>9</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="9" t="s">
@@ -1170,12 +1170,12 @@
         <v>10</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
@@ -1187,7 +1187,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9" t="s">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>24</v>
@@ -1209,19 +1209,19 @@
         <v>16</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="9"/>
       <c r="F14" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I14" s="9"/>
       <c r="AJ14" s="16"/>
@@ -1231,50 +1231,42 @@
         <v>17</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I15" s="9"/>
       <c r="AJ15" s="16"/>
     </row>
-    <row r="16" spans="1:40" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>27</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="9"/>
       <c r="F16" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>27</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
       <c r="I16" s="9"/>
       <c r="AJ16" s="16"/>
     </row>
@@ -1283,15 +1275,15 @@
         <v>19</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>24</v>
@@ -1333,52 +1325,52 @@
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A20" s="35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="35" t="s">
-        <v>42</v>
-      </c>
       <c r="D20" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="35" t="s">
+      <c r="I20" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="J20" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="K20" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="L20" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="M20" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="N20" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="F20" s="35" t="s">
+      <c r="O20" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="G20" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="H20" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="I20" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="J20" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="K20" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="L20" s="35" t="s">
+      <c r="P20" s="35" t="s">
         <v>54</v>
-      </c>
-      <c r="M20" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="N20" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="O20" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="P20" s="35" t="s">
-        <v>55</v>
       </c>
       <c r="Q20" s="16"/>
       <c r="R20" s="16"/>
@@ -1436,7 +1428,7 @@
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A22" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" s="25">
         <v>11</v>
@@ -1460,7 +1452,7 @@
         <v>0.99906479999999998</v>
       </c>
       <c r="I22" s="27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J22" s="32">
         <v>12</v>
@@ -1588,7 +1580,7 @@
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A25" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" s="25">
         <v>2</v>
@@ -1612,7 +1604,7 @@
         <v>0.99996700000000005</v>
       </c>
       <c r="I25" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J25" s="32">
         <v>2</v>
@@ -1838,7 +1830,7 @@
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A30" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B30" s="25">
         <v>4</v>
@@ -1862,7 +1854,7 @@
         <v>1</v>
       </c>
       <c r="I30" s="27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J30" s="32">
         <v>5</v>
@@ -2160,8 +2152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EDC67C0-1A4E-5E4D-A31E-90F1C836F6D0}">
   <dimension ref="A4:U29"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2180,10 +2172,10 @@
     </row>
     <row r="5" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="41" t="s">
         <v>5</v>
@@ -2210,10 +2202,10 @@
         <v>12</v>
       </c>
       <c r="L5" s="42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>5</v>
@@ -2245,7 +2237,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>22</v>
@@ -2254,13 +2246,13 @@
         <v>24</v>
       </c>
       <c r="H6" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L6">
         <v>1</v>
       </c>
       <c r="M6" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N6" t="s">
         <v>22</v>
@@ -2269,13 +2261,13 @@
         <v>24</v>
       </c>
       <c r="R6" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T6" t="s">
         <v>24</v>
       </c>
       <c r="U6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
@@ -2283,7 +2275,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" s="22" t="s">
         <v>22</v>
@@ -2292,16 +2284,16 @@
         <v>24</v>
       </c>
       <c r="G7" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H7" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L7">
         <v>2</v>
       </c>
       <c r="M7" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N7" t="s">
         <v>22</v>
@@ -2310,16 +2302,16 @@
         <v>24</v>
       </c>
       <c r="R7" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S7" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T7" t="s">
         <v>24</v>
       </c>
       <c r="U7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
@@ -2327,7 +2319,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" s="22" t="s">
         <v>22</v>
@@ -2336,19 +2328,19 @@
         <v>24</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G8" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H8" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L8">
         <v>3</v>
       </c>
       <c r="M8" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N8" t="s">
         <v>22</v>
@@ -2357,19 +2349,19 @@
         <v>26</v>
       </c>
       <c r="P8" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R8" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S8" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T8" t="s">
         <v>24</v>
       </c>
       <c r="U8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
@@ -2377,7 +2369,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>22</v>
@@ -2386,38 +2378,38 @@
         <v>26</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G9" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H9" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J9" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K9" s="37"/>
       <c r="L9">
         <v>3</v>
       </c>
       <c r="M9" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N9" t="s">
         <v>26</v>
       </c>
       <c r="O9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R9" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S9" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U9" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
@@ -2425,32 +2417,32 @@
         <v>5</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G10" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H10" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J10" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K10" s="37"/>
       <c r="L10">
         <v>4</v>
       </c>
       <c r="M10" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N10" t="s">
         <v>22</v>
@@ -2459,22 +2451,22 @@
         <v>26</v>
       </c>
       <c r="P10" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q10" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R10" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S10" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T10" t="s">
         <v>24</v>
       </c>
       <c r="U10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
@@ -2482,56 +2474,56 @@
         <v>5</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C11" s="22" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
         <v>24</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G11" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H11" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J11" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K11" s="37"/>
       <c r="L11">
         <v>5</v>
       </c>
       <c r="M11" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N11" t="s">
         <v>22</v>
       </c>
       <c r="P11" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q11" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R11" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S11" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T11" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
@@ -2539,7 +2531,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="22" t="s">
         <v>22</v>
@@ -2548,47 +2540,47 @@
         <v>26</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G12" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H12" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I12" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J12" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K12" s="37"/>
       <c r="L12">
         <v>5</v>
       </c>
       <c r="M12" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N12" t="s">
         <v>22</v>
       </c>
       <c r="O12" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P12" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q12" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R12" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S12" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
@@ -2596,56 +2588,56 @@
         <v>6</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" s="22" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
         <v>26</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G13" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H13" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I13" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J13" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K13" s="37"/>
       <c r="L13">
         <v>5</v>
       </c>
       <c r="M13" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N13" t="s">
         <v>22</v>
       </c>
       <c r="P13" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q13" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R13" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S13" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U13" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
@@ -2656,132 +2648,132 @@
         <v>22</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F14" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G14" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H14" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I14" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J14" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K14" s="37"/>
       <c r="L14">
         <v>6</v>
       </c>
       <c r="M14" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N14" t="s">
         <v>22</v>
       </c>
       <c r="P14" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q14" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R14" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S14" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T14" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U14" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B15" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="D15" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="E15" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="F15" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="G15" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="H15" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="23" t="s">
+      <c r="I15" s="23" t="s">
         <v>46</v>
-      </c>
-      <c r="I15" s="23" t="s">
-        <v>47</v>
       </c>
       <c r="L15">
         <v>6</v>
       </c>
       <c r="M15" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N15" t="s">
         <v>22</v>
       </c>
       <c r="P15" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q15" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R15" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S15" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T15" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B16" s="35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="35" t="s">
-        <v>42</v>
-      </c>
       <c r="E16" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="I16" s="35" t="s">
         <v>54</v>
-      </c>
-      <c r="F16" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="G16" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="H16" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="I16" s="35" t="s">
-        <v>55</v>
       </c>
       <c r="L16">
         <v>7</v>
@@ -2793,30 +2785,30 @@
         <v>22</v>
       </c>
       <c r="O16" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P16" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q16" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R16" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S16" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T16" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U16" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B17" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" s="27">
         <v>5</v>
@@ -2842,7 +2834,7 @@
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B18" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" s="27">
         <v>4</v>
@@ -2866,33 +2858,33 @@
         <v>0.71017669999999999</v>
       </c>
       <c r="M18" s="35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N18" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="O18" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="O18" s="35" t="s">
-        <v>42</v>
-      </c>
       <c r="P18" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q18" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="R18" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="S18" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="T18" s="35" t="s">
         <v>54</v>
-      </c>
-      <c r="Q18" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="R18" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="S18" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="T18" s="35" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B19" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19" s="27">
         <v>6</v>
@@ -2916,7 +2908,7 @@
         <v>0.8301193</v>
       </c>
       <c r="M19" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N19" s="25">
         <v>8</v>
@@ -2942,7 +2934,7 @@
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B20" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C20" s="27">
         <v>5</v>
@@ -2966,7 +2958,7 @@
         <v>0.93834240000000002</v>
       </c>
       <c r="M20" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N20" s="25">
         <v>9</v>
@@ -3016,7 +3008,7 @@
         <v>0.96080239999999995</v>
       </c>
       <c r="M21" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N21" s="25">
         <v>6</v>
@@ -3042,7 +3034,7 @@
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B22" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" s="27">
         <v>4</v>
@@ -3066,7 +3058,7 @@
         <v>0.97994009999999998</v>
       </c>
       <c r="M22" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N22" s="25">
         <v>7</v>
@@ -3092,7 +3084,7 @@
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B23" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C23" s="27">
         <v>8</v>
@@ -3142,7 +3134,7 @@
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B24" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C24" s="27">
         <v>5</v>
@@ -3166,7 +3158,7 @@
         <v>0.99723709999999999</v>
       </c>
       <c r="M24" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N24" s="25">
         <v>7</v>
@@ -3192,7 +3184,7 @@
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B25" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C25" s="27">
         <v>9</v>
@@ -3216,7 +3208,7 @@
         <v>0.99939679999999997</v>
       </c>
       <c r="M25" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N25" s="25">
         <v>10</v>
@@ -3242,7 +3234,7 @@
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B26" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C26" s="27">
         <v>10</v>
@@ -3266,7 +3258,7 @@
         <v>1</v>
       </c>
       <c r="M26" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N26" s="25">
         <v>4</v>
@@ -3292,7 +3284,7 @@
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.2">
       <c r="M27" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N27" s="25">
         <v>5</v>
@@ -3318,7 +3310,7 @@
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.2">
       <c r="M28" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N28" s="25">
         <v>11</v>
@@ -3344,7 +3336,7 @@
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.2">
       <c r="M29" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N29" s="25">
         <v>7</v>
@@ -3389,7 +3381,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -3402,7 +3394,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -3410,7 +3402,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -3418,21 +3410,21 @@
         <v>24</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="9"/>
       <c r="B6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -3440,7 +3432,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -3455,8 +3447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA9C2D77-AC9C-9448-AFB4-66C1E8246857}">
   <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView zoomScale="98" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3472,12 +3464,12 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -3516,28 +3508,28 @@
       <c r="I4" s="29"/>
       <c r="M4" s="23"/>
       <c r="N4" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="O4" s="23" t="s">
+      <c r="P4" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="P4" s="23" t="s">
+      <c r="Q4" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="Q4" s="23" t="s">
+      <c r="R4" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="R4" s="23" t="s">
+      <c r="S4" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="S4" s="23" t="s">
-        <v>45</v>
-      </c>
       <c r="T4" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U4" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="17" x14ac:dyDescent="0.2">
@@ -3609,7 +3601,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>22</v>
@@ -3619,7 +3611,7 @@
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>22</v>
@@ -3637,7 +3629,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>26</v>
@@ -3647,7 +3639,7 @@
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>24</v>
@@ -3665,14 +3657,14 @@
         <v>7</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>26</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -3686,12 +3678,12 @@
         <v>8</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="9" t="s">
@@ -3707,12 +3699,12 @@
         <v>9</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="9" t="s">
@@ -3728,12 +3720,12 @@
         <v>10</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
@@ -3747,7 +3739,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9" t="s">
@@ -3755,10 +3747,10 @@
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
@@ -3771,18 +3763,18 @@
         <v>16</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="9"/>
       <c r="F14" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I14" s="9"/>
       <c r="M14" s="24">
@@ -3794,15 +3786,15 @@
         <v>17</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="20"/>
       <c r="F15" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G15" s="13" t="s">
         <v>24</v>
@@ -3818,14 +3810,14 @@
         <v>18</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>26</v>
@@ -3835,7 +3827,7 @@
       </c>
       <c r="I16" s="9"/>
       <c r="M16" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
@@ -3843,12 +3835,12 @@
         <v>19</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
@@ -3856,7 +3848,7 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
@@ -3883,81 +3875,81 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C22" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="35" t="s">
-        <v>57</v>
-      </c>
       <c r="E22" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="35" t="s">
-        <v>42</v>
-      </c>
       <c r="G22" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="H22" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="I22" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="J22" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="K22" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="H22" s="35" t="s">
+      <c r="L22" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="M22" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="N22" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="O22" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="P22" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q22" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="R22" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="S22" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="I22" s="35" t="s">
+      <c r="T22" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="J22" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="K22" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="L22" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="M22" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="N22" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="O22" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="P22" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q22" s="35" t="s">
+      <c r="U22" s="35" t="s">
         <v>54</v>
-      </c>
-      <c r="R22" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="S22" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="T22" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="U22" s="35" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E23" s="25">
         <v>11</v>
@@ -3981,13 +3973,13 @@
         <v>0.99999970000000005</v>
       </c>
       <c r="L23" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M23" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N23" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O23" s="25">
         <v>12</v>
@@ -4016,10 +4008,10 @@
         <v>5</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E24" s="25">
         <v>3</v>
@@ -4046,10 +4038,10 @@
         <v>5</v>
       </c>
       <c r="M24" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N24" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O24" s="25">
         <v>3</v>
@@ -4078,10 +4070,10 @@
         <v>6</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E25" s="25">
         <v>3</v>
@@ -4108,10 +4100,10 @@
         <v>9</v>
       </c>
       <c r="M25" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N25" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O25" s="25">
         <v>3</v>
@@ -4140,10 +4132,10 @@
         <v>11</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E26" s="25">
         <v>3</v>
@@ -4170,10 +4162,10 @@
         <v>10</v>
       </c>
       <c r="M26" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N26" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O26" s="25">
         <v>3</v>
@@ -4202,10 +4194,10 @@
         <v>10</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E27" s="25">
         <v>3</v>
@@ -4232,10 +4224,10 @@
         <v>6</v>
       </c>
       <c r="M27" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N27" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O27" s="25">
         <v>3</v>
@@ -4264,10 +4256,10 @@
         <v>9</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E28" s="25">
         <v>3</v>
@@ -4291,13 +4283,13 @@
         <v>1</v>
       </c>
       <c r="L28" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M28" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N28" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O28" s="25">
         <v>5</v>
@@ -4323,13 +4315,13 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B29" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E29" s="25">
         <v>2</v>
@@ -4356,10 +4348,10 @@
         <v>8</v>
       </c>
       <c r="M29" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N29" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O29" s="25">
         <v>3</v>
@@ -4388,10 +4380,10 @@
         <v>8</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E30" s="25">
         <v>3</v>
@@ -4415,13 +4407,13 @@
         <v>1</v>
       </c>
       <c r="L30" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M30" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N30" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O30" s="25">
         <v>2</v>
@@ -4450,10 +4442,10 @@
         <v>7</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E31" s="25">
         <v>3</v>
@@ -4480,10 +4472,10 @@
         <v>7</v>
       </c>
       <c r="M31" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N31" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O31" s="25">
         <v>3</v>
@@ -4509,13 +4501,13 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B32" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E32" s="25">
         <v>4</v>
@@ -4542,10 +4534,10 @@
         <v>11</v>
       </c>
       <c r="M32" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N32" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O32" s="25">
         <v>3</v>
@@ -4571,75 +4563,75 @@
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B33" s="35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C33" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="D33" s="35" t="s">
-        <v>57</v>
-      </c>
       <c r="E33" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F33" s="35" t="s">
-        <v>42</v>
-      </c>
       <c r="G33" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="H33" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="I33" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="J33" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="K33" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="H33" s="35" t="s">
+      <c r="L33" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="M33" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="N33" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="O33" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="P33" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q33" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="R33" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="S33" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="I33" s="35" t="s">
+      <c r="T33" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="J33" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="K33" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="L33" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="M33" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="N33" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="O33" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="P33" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q33" s="35" t="s">
+      <c r="U33" s="35" t="s">
         <v>54</v>
-      </c>
-      <c r="R33" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="S33" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="T33" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="U33" s="35" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C34" s="40">
         <v>0.30498609999999998</v>
@@ -4793,7 +4785,7 @@
         <v>0.99717960000000005</v>
       </c>
       <c r="L36" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M36" s="25">
         <v>0.27425300000000002</v>
@@ -4949,7 +4941,7 @@
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B39" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -4979,7 +4971,7 @@
         <v>0.99983889999999997</v>
       </c>
       <c r="L39" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M39" s="25">
         <v>0</v>
@@ -5197,7 +5189,7 @@
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B43" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C43">
         <v>1.312206E-3</v>
@@ -5227,7 +5219,7 @@
         <v>1</v>
       </c>
       <c r="L43" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M43" s="25">
         <v>6.7467170000000007E-2</v>
@@ -5267,7 +5259,7 @@
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5280,7 +5272,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
@@ -5297,31 +5289,31 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="D2" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="E2" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="F2" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="G2" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="28" t="s">
-        <v>45</v>
-      </c>
       <c r="H2" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J2" s="25"/>
       <c r="K2" s="25"/>
@@ -5334,7 +5326,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" s="25">
         <v>7</v>
@@ -5368,7 +5360,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="25">
         <v>6</v>
@@ -5402,7 +5394,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C5" s="25">
         <v>7</v>
@@ -5436,7 +5428,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C6" s="25">
         <v>8</v>
@@ -5470,7 +5462,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C7" s="25">
         <v>5</v>
@@ -5504,7 +5496,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" s="25">
         <v>7</v>
@@ -5538,7 +5530,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C9" s="25">
         <v>10</v>
@@ -5572,7 +5564,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C10" s="25">
         <v>11</v>
@@ -5606,7 +5598,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" s="25">
         <v>7</v>
@@ -5640,7 +5632,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" s="25">
         <v>5</v>
@@ -5674,7 +5666,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C13" s="25">
         <v>12</v>
@@ -5915,7 +5907,9 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="25"/>
-      <c r="B26" s="25"/>
+      <c r="B26" s="25" t="s">
+        <v>102</v>
+      </c>
       <c r="C26" s="25"/>
       <c r="D26" s="25"/>
       <c r="E26" s="25"/>

</xml_diff>